<commit_message>
& №39293 от 28.03.2024 numizm.at
</commit_message>
<xml_diff>
--- a/Collections/EURO/France/#EURO#France#Commemorative#[2007-present]#UNC%varieties.xlsx
+++ b/Collections/EURO/France/#EURO#France#Commemorative#[2007-present]#UNC%varieties.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lord_Alexator\Documents\CoinCollection\Collections\EURO\France\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{396EC8C4-EE57-415F-9D01-4DB755A69F1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4365AE89-ABB6-43A8-9E95-32F9E52BDF5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4180" yWindow="3860" windowWidth="28800" windowHeight="17740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2€" sheetId="1" r:id="rId1"/>
@@ -400,7 +400,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -467,6 +467,13 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -602,7 +609,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -686,13 +693,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Гиперссылка" xfId="2" builtinId="8"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
     <cellStyle name="Обычный 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
-  <dxfs count="21">
+  <dxfs count="22">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF9BE5FF"/>
+          <bgColor rgb="FF9BE5FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -867,9 +885,9 @@
     <filterColumn colId="2" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="№" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Link" dataDxfId="1" dataCellStyle="Гиперссылка"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Description (single table, table set, mintage, prices):" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="№" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Link" dataDxfId="2" dataCellStyle="Гиперссылка"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Description (single table, table set, mintage, prices):" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="1" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -1144,7 +1162,7 @@
       <pane xSplit="10" ySplit="2" topLeftCell="K3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B1" sqref="B1:B2"/>
+      <selection pane="bottomRight" activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1993,10 +2011,10 @@
         <v>78</v>
       </c>
       <c r="G29" s="7"/>
-      <c r="H29" s="19" t="s">
+      <c r="H29" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="I29" s="8">
+      <c r="I29" s="31">
         <v>0</v>
       </c>
       <c r="J29" s="9" t="str">
@@ -2080,10 +2098,10 @@
         <v>78</v>
       </c>
       <c r="G32" s="7"/>
-      <c r="H32" s="19" t="s">
+      <c r="H32" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="I32" s="8">
+      <c r="I32" s="31">
         <v>0</v>
       </c>
       <c r="J32" s="9" t="str">
@@ -2140,7 +2158,7 @@
         <v>79</v>
       </c>
       <c r="G34" s="7"/>
-      <c r="H34" s="19" t="s">
+      <c r="H34" s="23" t="s">
         <v>89</v>
       </c>
       <c r="I34" s="8">
@@ -2229,10 +2247,10 @@
         <v>79</v>
       </c>
       <c r="G37" s="7"/>
-      <c r="H37" s="19" t="s">
+      <c r="H37" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="I37" s="8">
+      <c r="I37" s="31">
         <v>0</v>
       </c>
       <c r="J37" s="9" t="str">
@@ -2260,10 +2278,10 @@
         <v>79</v>
       </c>
       <c r="G38" s="7"/>
-      <c r="H38" s="19" t="s">
+      <c r="H38" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="I38" s="8">
+      <c r="I38" s="31">
         <v>0</v>
       </c>
       <c r="J38" s="9" t="str">
@@ -2307,11 +2325,11 @@
     <mergeCell ref="C1:G1"/>
   </mergeCells>
   <conditionalFormatting sqref="I3 I6 I10 I12 I14 I17 I21 I23 I26 I8">
-    <cfRule type="containsText" dxfId="20" priority="59" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="21" priority="59" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(I3))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I3 I6 I10 I12 I14 I17 I21 I23 I26 I8">
+  <conditionalFormatting sqref="I6 I3 I10 I12 I14 I17 I21 I23 I26 I8">
     <cfRule type="colorScale" priority="60">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -2324,11 +2342,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4 I7 I9 I11 I13 I16 I19 I22 I25 I28 I30">
-    <cfRule type="containsText" dxfId="19" priority="51" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="20" priority="51" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(I4))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I4 I7 I9 I11 I13 I16 I19 I22 I25 I28 I30">
+  <conditionalFormatting sqref="I7 I4 I9 I11 I13 I16 I19 I22 I25 I28 I30">
     <cfRule type="colorScale" priority="52">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -2341,7 +2359,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5">
-    <cfRule type="containsText" dxfId="18" priority="39" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="19" priority="39" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(I5))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2358,7 +2376,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I15">
-    <cfRule type="containsText" dxfId="17" priority="37" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="18" priority="37" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(I15))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2375,7 +2393,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I18">
-    <cfRule type="containsText" dxfId="16" priority="33" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="17" priority="33" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(I18))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2392,12 +2410,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I20">
-    <cfRule type="containsText" dxfId="15" priority="31" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="16" priority="31" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(I20))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I24">
-    <cfRule type="containsText" dxfId="14" priority="29" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="15" priority="29" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(I24))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2426,7 +2444,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I27">
-    <cfRule type="containsText" dxfId="13" priority="27" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="14" priority="27" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(I27))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2443,7 +2461,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I31">
-    <cfRule type="containsText" dxfId="12" priority="25" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="13" priority="25" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(I31))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2460,7 +2478,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I38">
-    <cfRule type="containsText" dxfId="11" priority="3" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="12" priority="3" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(I38))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2477,7 +2495,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I29">
-    <cfRule type="containsText" dxfId="10" priority="19" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="11" priority="19" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(I29))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2494,7 +2512,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I32">
-    <cfRule type="containsText" dxfId="9" priority="17" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="10" priority="17" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(I32))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2511,7 +2529,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I33">
-    <cfRule type="containsText" dxfId="8" priority="15" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="9" priority="15" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(I33))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2528,7 +2546,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I34">
-    <cfRule type="containsText" dxfId="7" priority="13" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="8" priority="13" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(I34))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2545,7 +2563,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I35">
-    <cfRule type="containsText" dxfId="6" priority="11" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="7" priority="11" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(I35))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2562,7 +2580,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I39">
-    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="6" priority="1" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(I39))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2579,7 +2597,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I36">
-    <cfRule type="containsText" dxfId="4" priority="7" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="5" priority="7" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(I36))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2596,7 +2614,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I37">
-    <cfRule type="containsText" dxfId="3" priority="5" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(I37))))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>